<commit_message>
deployment for release v2.3
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ErrorFiles/dementia_Freiburg_v1.xlsx
+++ b/src/main/resources/data/ErrorFiles/dementia_Freiburg_v1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -85,9 +85,6 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/PID_PSEUDONYMOUS</t>
-  </si>
-  <si>
     <t xml:space="preserve">SEX</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">/root/EXAMINATION_DATE</t>
-  </si>
-  <si>
     <t xml:space="preserve">YEAR_OF_BIRTH</t>
   </si>
   <si>
@@ -208,10 +202,10 @@
     <t xml:space="preserve">How old is the patient in years.</t>
   </si>
   <si>
-    <t xml:space="preserve">[stays the same],  ,[corresponds to one of the groups: {“-50y”},{”50-59y”},{”60-69y”},{”70-79y”},{”+80y”}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subjectageyears,  agegroup</t>
+    <t xml:space="preserve">{stays the same}, {AGE*12}, {corresponds to one of the groups: {“-50y”},{”50-59y”},{”60-69y”},{”70-79y”},{”+80y”}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subjectageyears, subjectage, agegroup</t>
   </si>
   <si>
     <t xml:space="preserve">ALZHEIMER_BROAD_CATEGORY</t>
@@ -424,25 +418,25 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="53.0510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,9 +529,6 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
@@ -547,31 +538,31 @@
         <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="I4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,24 +570,21 @@
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
@@ -605,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>15</v>
@@ -616,12 +604,12 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -632,32 +620,32 @@
         <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -665,25 +653,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -694,27 +682,27 @@
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -725,27 +713,27 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -756,27 +744,27 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -787,27 +775,27 @@
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -818,27 +806,27 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -849,27 +837,27 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -880,10 +868,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>15</v>
@@ -891,14 +879,14 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -909,32 +897,32 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="9"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="61.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -942,34 +930,34 @@
         <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>